<commit_message>
melhorias no classificador e ajustes na planilha
</commit_message>
<xml_diff>
--- a/airfryer.xlsx
+++ b/airfryer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14d65f97922bf1aa/Área de Trabalho/INSPER/2° sem/C dados/Projeto1- Cdados/Proj1Cdados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1118" documentId="11_CA44DC90CA32E62EC7C03AD4197D333511A52485" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{193273CD-62C6-4A66-BDCD-166E93397C99}"/>
+  <xr:revisionPtr revIDLastSave="1141" documentId="11_CA44DC90CA32E62EC7C03AD4197D333511A52485" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B7BAC8-2DFD-4956-9260-F1E7BA219E33}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2120,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A306" sqref="A306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2838,7 +2838,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -2854,7 +2854,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -2958,7 +2958,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -3134,7 +3134,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -3206,7 +3206,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -3870,7 +3870,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
@@ -4422,7 +4422,7 @@
         <v>278</v>
       </c>
       <c r="B279">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
@@ -4610,8 +4610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="B166" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4665,7 +4665,7 @@
         <v>306</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -4681,7 +4681,7 @@
         <v>308</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -4729,7 +4729,7 @@
         <v>314</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -4745,7 +4745,7 @@
         <v>316</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -4937,7 +4937,7 @@
         <v>340</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -5265,7 +5265,7 @@
         <v>381</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="29" x14ac:dyDescent="0.35">
@@ -5313,7 +5313,7 @@
         <v>387</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -5337,7 +5337,7 @@
         <v>390</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -5465,7 +5465,7 @@
         <v>406</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -5529,7 +5529,7 @@
         <v>414</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -5737,7 +5737,7 @@
         <v>440</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -5745,7 +5745,7 @@
         <v>441</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -5865,7 +5865,7 @@
         <v>456</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -6033,7 +6033,7 @@
         <v>477</v>
       </c>
       <c r="B177">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -6121,7 +6121,7 @@
         <v>488</v>
       </c>
       <c r="B188">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -6161,7 +6161,7 @@
         <v>493</v>
       </c>
       <c r="B193">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>